<commit_message>
reinsurer sahe into account
</commit_message>
<xml_diff>
--- a/examples/programs/aviation_axa_xl_2024.xlsx
+++ b/examples/programs/aviation_axa_xl_2024.xlsx
@@ -657,7 +657,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>cession_rate</t>
+          <t>cession_PCT</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -879,10 +879,10 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
         <v>65</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>0.05</v>
@@ -910,10 +910,10 @@
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
         <v>65</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>0.05</v>
@@ -941,10 +941,10 @@
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
         <v>65</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>0.05</v>
@@ -972,10 +972,10 @@
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
         <v>65</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
       </c>
       <c r="E10" t="n">
         <v>0.05</v>
@@ -1003,10 +1003,10 @@
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="n">
+        <v>65</v>
+      </c>
+      <c r="D11" t="n">
         <v>50</v>
-      </c>
-      <c r="D11" t="n">
-        <v>65</v>
       </c>
       <c r="E11" t="n">
         <v>0.05</v>
@@ -1034,10 +1034,10 @@
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="n">
+        <v>65</v>
+      </c>
+      <c r="D12" t="n">
         <v>50</v>
-      </c>
-      <c r="D12" t="n">
-        <v>65</v>
       </c>
       <c r="E12" t="n">
         <v>0.05</v>
@@ -1065,10 +1065,10 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
+        <v>65</v>
+      </c>
+      <c r="D13" t="n">
         <v>50</v>
-      </c>
-      <c r="D13" t="n">
-        <v>65</v>
       </c>
       <c r="E13" t="n">
         <v>0.05</v>
@@ -1096,10 +1096,10 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
+        <v>65</v>
+      </c>
+      <c r="D14" t="n">
         <v>50</v>
-      </c>
-      <c r="D14" t="n">
-        <v>65</v>
       </c>
       <c r="E14" t="n">
         <v>0.05</v>
@@ -1127,10 +1127,10 @@
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="n">
+        <v>115</v>
+      </c>
+      <c r="D15" t="n">
         <v>100</v>
-      </c>
-      <c r="D15" t="n">
-        <v>115</v>
       </c>
       <c r="E15" t="n">
         <v>0.05</v>
@@ -1158,10 +1158,10 @@
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="n">
+        <v>115</v>
+      </c>
+      <c r="D16" t="n">
         <v>100</v>
-      </c>
-      <c r="D16" t="n">
-        <v>115</v>
       </c>
       <c r="E16" t="n">
         <v>0.05</v>
@@ -1189,10 +1189,10 @@
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="n">
+        <v>115</v>
+      </c>
+      <c r="D17" t="n">
         <v>100</v>
-      </c>
-      <c r="D17" t="n">
-        <v>115</v>
       </c>
       <c r="E17" t="n">
         <v>0.05</v>
@@ -1220,10 +1220,10 @@
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="n">
+        <v>115</v>
+      </c>
+      <c r="D18" t="n">
         <v>100</v>
-      </c>
-      <c r="D18" t="n">
-        <v>115</v>
       </c>
       <c r="E18" t="n">
         <v>0.05</v>
@@ -1251,10 +1251,10 @@
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="n">
+        <v>215</v>
+      </c>
+      <c r="D19" t="n">
         <v>100</v>
-      </c>
-      <c r="D19" t="n">
-        <v>215</v>
       </c>
       <c r="E19" t="n">
         <v>0.05</v>
@@ -1282,10 +1282,10 @@
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="n">
+        <v>215</v>
+      </c>
+      <c r="D20" t="n">
         <v>100</v>
-      </c>
-      <c r="D20" t="n">
-        <v>215</v>
       </c>
       <c r="E20" t="n">
         <v>0.05</v>
@@ -1313,10 +1313,10 @@
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="n">
+        <v>215</v>
+      </c>
+      <c r="D21" t="n">
         <v>100</v>
-      </c>
-      <c r="D21" t="n">
-        <v>215</v>
       </c>
       <c r="E21" t="n">
         <v>0.05</v>
@@ -1344,10 +1344,10 @@
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="n">
+        <v>215</v>
+      </c>
+      <c r="D22" t="n">
         <v>100</v>
-      </c>
-      <c r="D22" t="n">
-        <v>215</v>
       </c>
       <c r="E22" t="n">
         <v>0.05</v>
@@ -1375,10 +1375,10 @@
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="n">
+        <v>315</v>
+      </c>
+      <c r="D23" t="n">
         <v>100</v>
-      </c>
-      <c r="D23" t="n">
-        <v>315</v>
       </c>
       <c r="E23" t="n">
         <v>0.05</v>
@@ -1406,10 +1406,10 @@
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="n">
+        <v>315</v>
+      </c>
+      <c r="D24" t="n">
         <v>100</v>
-      </c>
-      <c r="D24" t="n">
-        <v>315</v>
       </c>
       <c r="E24" t="n">
         <v>0.05</v>
@@ -1437,10 +1437,10 @@
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="n">
+        <v>315</v>
+      </c>
+      <c r="D25" t="n">
         <v>100</v>
-      </c>
-      <c r="D25" t="n">
-        <v>315</v>
       </c>
       <c r="E25" t="n">
         <v>0.05</v>
@@ -1468,10 +1468,10 @@
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="n">
+        <v>315</v>
+      </c>
+      <c r="D26" t="n">
         <v>100</v>
-      </c>
-      <c r="D26" t="n">
-        <v>315</v>
       </c>
       <c r="E26" t="n">
         <v>0.05</v>
@@ -1499,10 +1499,10 @@
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="n">
+        <v>415</v>
+      </c>
+      <c r="D27" t="n">
         <v>150</v>
-      </c>
-      <c r="D27" t="n">
-        <v>415</v>
       </c>
       <c r="E27" t="n">
         <v>0.05</v>
@@ -1530,10 +1530,10 @@
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="n">
+        <v>415</v>
+      </c>
+      <c r="D28" t="n">
         <v>150</v>
-      </c>
-      <c r="D28" t="n">
-        <v>415</v>
       </c>
       <c r="E28" t="n">
         <v>0.05</v>
@@ -1561,10 +1561,10 @@
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="n">
+        <v>415</v>
+      </c>
+      <c r="D29" t="n">
         <v>150</v>
-      </c>
-      <c r="D29" t="n">
-        <v>415</v>
       </c>
       <c r="E29" t="n">
         <v>0.05</v>
@@ -1592,10 +1592,10 @@
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="n">
+        <v>415</v>
+      </c>
+      <c r="D30" t="n">
         <v>150</v>
-      </c>
-      <c r="D30" t="n">
-        <v>415</v>
       </c>
       <c r="E30" t="n">
         <v>0.05</v>
@@ -1623,10 +1623,10 @@
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="n">
+        <v>23.333333</v>
+      </c>
+      <c r="D31" t="n">
         <v>43.333333</v>
-      </c>
-      <c r="D31" t="n">
-        <v>23.333333</v>
       </c>
       <c r="E31" t="n">
         <v>0.05</v>
@@ -1654,10 +1654,10 @@
       </c>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="n">
+        <v>43.333333</v>
+      </c>
+      <c r="D32" t="n">
         <v>33.333333</v>
-      </c>
-      <c r="D32" t="n">
-        <v>43.333333</v>
       </c>
       <c r="E32" t="n">
         <v>0.05</v>
@@ -1685,10 +1685,10 @@
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="n">
+        <v>76.66666600000001</v>
+      </c>
+      <c r="D33" t="n">
         <v>66.66666600000001</v>
-      </c>
-      <c r="D33" t="n">
-        <v>76.66666600000001</v>
       </c>
       <c r="E33" t="n">
         <v>0.05</v>
@@ -1716,10 +1716,10 @@
       </c>
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="n">
+        <v>143.333333</v>
+      </c>
+      <c r="D34" t="n">
         <v>66.66666600000001</v>
-      </c>
-      <c r="D34" t="n">
-        <v>143.333333</v>
       </c>
       <c r="E34" t="n">
         <v>0.05</v>
@@ -1747,10 +1747,10 @@
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="n">
+        <v>210</v>
+      </c>
+      <c r="D35" t="n">
         <v>66.66666600000001</v>
-      </c>
-      <c r="D35" t="n">
-        <v>210</v>
       </c>
       <c r="E35" t="n">
         <v>0.05</v>
@@ -1778,10 +1778,10 @@
       </c>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="n">
+        <v>276.666666</v>
+      </c>
+      <c r="D36" t="n">
         <v>100</v>
-      </c>
-      <c r="D36" t="n">
-        <v>276.666666</v>
       </c>
       <c r="E36" t="n">
         <v>0.05</v>

</xml_diff>

<commit_message>
data model for program
</commit_message>
<xml_diff>
--- a/examples/programs/aviation_axa_xl_2024.xlsx
+++ b/examples/programs/aviation_axa_xl_2024.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,16 +438,98 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>program_name</t>
+          <t>REPROG_ID_PRE</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>REPROG_TITLE</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>CED_ID_PRE</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>CED_NAME_PRE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>REPROG_ACTIVE_IND</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>REPROG_COMMENT</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>REPROG_UW_DEPARTMENT_CD</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>REPROG_UW_DEPARTMENT_NAME</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>REPROG_UW_DEPARTMENT_LOB_CD</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>REPROG_UW_DEPARTMENT_LOB_NAME</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>BUSPAR_CED_REG_CLASS_CD</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>BUSPAR_CED_REG_CLASS_NAME</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>REPROG_MAIN_CURRENCY_CD</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>REPROG_MANAGEMENT_REPORTING_LOB_CD</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>AVIATION_AXA_XL_2024</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
data model of structures
</commit_message>
<xml_diff>
--- a/examples/programs/aviation_axa_xl_2024.xlsx
+++ b/examples/programs/aviation_axa_xl_2024.xlsx
@@ -542,7 +542,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -553,164 +553,398 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>structure_name</t>
+          <t>INSPER_ID_PRE</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>contract_order</t>
+          <t>BUSINESS_ID_PRE</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>type_of_participation</t>
+          <t>TYPE_OF_PARTICIPATION_CD</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>claim_basis</t>
+          <t>TYPE_OF_INSURED_PERIOD_CD</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ACTIVE_FLAG_CD</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>INSPER_EFFECTIVE_DATE</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>INSPER_EXPIRY_DATE</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>REPROG_ID_PRE</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>BUSINESS_TITLE</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>INSPER_LAYER_NO</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>INSPER_MAIN_CURRENCY_CD</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>INSPER_UW_YEAR</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>INSPER_CONTRACT_ORDER</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>INSPER_CONTRACT_FORM_CD_SLAV</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>INSPER_CONTRACT_LODRA_CD_SLAV</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>INSPER_CONTRACT_COVERAGE_CD_SLAV</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>INSPER_CLAIM_BASIS_CD</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>INSPER_LODRA_CD_SLAV</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>INSPER_LOD_TO_RA_DATE_SLAV</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>INSPER_COMMENT</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>quota_share</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>QS_1</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>quota_share</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr">
         <is>
           <t>risk_attaching</t>
         </is>
       </c>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>excess_of_loss</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>XOL_1</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
         <v>1</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>risk_attaching</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
         <is>
           <t>excess_of_loss</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>XOL_2</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>2</v>
+      </c>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr">
         <is>
           <t>risk_attaching</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>XOL_2</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="inlineStr">
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
         <is>
           <t>excess_of_loss</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>XOL_3</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>3</v>
+      </c>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr">
         <is>
           <t>risk_attaching</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>XOL_3</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
         <is>
           <t>excess_of_loss</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>XOL_4</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>4</v>
+      </c>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr">
         <is>
           <t>risk_attaching</t>
         </is>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>XOL_4</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>4</v>
-      </c>
-      <c r="C6" t="inlineStr">
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
         <is>
           <t>excess_of_loss</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>XOL_5</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>5</v>
+      </c>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr">
         <is>
           <t>risk_attaching</t>
         </is>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>XOL_5</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C7" t="inlineStr">
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
         <is>
           <t>excess_of_loss</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>XOL_6</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>6</v>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr">
         <is>
           <t>risk_attaching</t>
         </is>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>XOL_6</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>6</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>excess_of_loss</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>risk_attaching</t>
-        </is>
-      </c>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -734,7 +968,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>structure_name</t>
+          <t>BUSINESS_TITLE</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">

</xml_diff>

<commit_message>
better program creation to excel
</commit_message>
<xml_diff>
--- a/examples/programs/aviation_axa_xl_2024.xlsx
+++ b/examples/programs/aviation_axa_xl_2024.xlsx
@@ -1391,18 +1391,18 @@
         <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="Q11" t="n">
-        <v>50000000</v>
+        <v>43333333</v>
       </c>
       <c r="S11" t="n">
-        <v>65000000</v>
+        <v>23333333</v>
       </c>
       <c r="AH11" t="n">
         <v>0.05</v>
@@ -1420,7 +1420,7 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>CAD</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="Q12" t="n">
@@ -1445,7 +1445,7 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>CAD</t>
         </is>
       </c>
       <c r="Q13" t="n">
@@ -1470,7 +1470,7 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="Q14" t="n">
@@ -1491,18 +1491,18 @@
         <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="Q15" t="n">
-        <v>100000000</v>
+        <v>50000000</v>
       </c>
       <c r="S15" t="n">
-        <v>115000000</v>
+        <v>65000000</v>
       </c>
       <c r="AH15" t="n">
         <v>0.05</v>
@@ -1516,18 +1516,18 @@
         <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>CAD</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="Q16" t="n">
-        <v>100000000</v>
+        <v>33333333</v>
       </c>
       <c r="S16" t="n">
-        <v>115000000</v>
+        <v>43333333</v>
       </c>
       <c r="AH16" t="n">
         <v>0.05</v>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="Q17" t="n">
@@ -1570,7 +1570,7 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>CAD</t>
         </is>
       </c>
       <c r="Q18" t="n">
@@ -1591,18 +1591,18 @@
         <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="Q19" t="n">
         <v>100000000</v>
       </c>
       <c r="S19" t="n">
-        <v>215000000</v>
+        <v>115000000</v>
       </c>
       <c r="AH19" t="n">
         <v>0.05</v>
@@ -1616,18 +1616,18 @@
         <v>1</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>CAD</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="Q20" t="n">
         <v>100000000</v>
       </c>
       <c r="S20" t="n">
-        <v>215000000</v>
+        <v>115000000</v>
       </c>
       <c r="AH20" t="n">
         <v>0.05</v>
@@ -1641,18 +1641,18 @@
         <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="Q21" t="n">
-        <v>100000000</v>
+        <v>66666666</v>
       </c>
       <c r="S21" t="n">
-        <v>215000000</v>
+        <v>76666666</v>
       </c>
       <c r="AH21" t="n">
         <v>0.05</v>
@@ -1670,7 +1670,7 @@
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="Q22" t="n">
@@ -1691,18 +1691,18 @@
         <v>1</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>CAD</t>
         </is>
       </c>
       <c r="Q23" t="n">
         <v>100000000</v>
       </c>
       <c r="S23" t="n">
-        <v>315000000</v>
+        <v>215000000</v>
       </c>
       <c r="AH23" t="n">
         <v>0.05</v>
@@ -1716,18 +1716,18 @@
         <v>1</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>CAD</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="Q24" t="n">
         <v>100000000</v>
       </c>
       <c r="S24" t="n">
-        <v>315000000</v>
+        <v>215000000</v>
       </c>
       <c r="AH24" t="n">
         <v>0.05</v>
@@ -1741,18 +1741,18 @@
         <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="Q25" t="n">
         <v>100000000</v>
       </c>
       <c r="S25" t="n">
-        <v>315000000</v>
+        <v>215000000</v>
       </c>
       <c r="AH25" t="n">
         <v>0.05</v>
@@ -1766,18 +1766,18 @@
         <v>1</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="Q26" t="n">
-        <v>100000000</v>
+        <v>66666666</v>
       </c>
       <c r="S26" t="n">
-        <v>315000000</v>
+        <v>143333333</v>
       </c>
       <c r="AH26" t="n">
         <v>0.05</v>
@@ -1791,7 +1791,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -1799,10 +1799,10 @@
         </is>
       </c>
       <c r="Q27" t="n">
-        <v>150000000</v>
+        <v>100000000</v>
       </c>
       <c r="S27" t="n">
-        <v>415000000</v>
+        <v>315000000</v>
       </c>
       <c r="AH27" t="n">
         <v>0.05</v>
@@ -1816,7 +1816,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -1824,10 +1824,10 @@
         </is>
       </c>
       <c r="Q28" t="n">
-        <v>150000000</v>
+        <v>100000000</v>
       </c>
       <c r="S28" t="n">
-        <v>415000000</v>
+        <v>315000000</v>
       </c>
       <c r="AH28" t="n">
         <v>0.05</v>
@@ -1841,7 +1841,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -1849,10 +1849,10 @@
         </is>
       </c>
       <c r="Q29" t="n">
-        <v>150000000</v>
+        <v>100000000</v>
       </c>
       <c r="S29" t="n">
-        <v>415000000</v>
+        <v>315000000</v>
       </c>
       <c r="AH29" t="n">
         <v>0.05</v>
@@ -1866,7 +1866,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -1874,10 +1874,10 @@
         </is>
       </c>
       <c r="Q30" t="n">
-        <v>150000000</v>
+        <v>100000000</v>
       </c>
       <c r="S30" t="n">
-        <v>415000000</v>
+        <v>315000000</v>
       </c>
       <c r="AH30" t="n">
         <v>0.05</v>
@@ -1891,7 +1891,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -1899,10 +1899,10 @@
         </is>
       </c>
       <c r="Q31" t="n">
-        <v>43333333</v>
+        <v>66666666</v>
       </c>
       <c r="S31" t="n">
-        <v>23333333</v>
+        <v>210000000</v>
       </c>
       <c r="AH31" t="n">
         <v>0.05</v>
@@ -1916,18 +1916,18 @@
         <v>1</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>GBP</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="Q32" t="n">
-        <v>33333333</v>
+        <v>150000000</v>
       </c>
       <c r="S32" t="n">
-        <v>43333333</v>
+        <v>415000000</v>
       </c>
       <c r="AH32" t="n">
         <v>0.05</v>
@@ -1941,18 +1941,18 @@
         <v>1</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>GBP</t>
+          <t>CAD</t>
         </is>
       </c>
       <c r="Q33" t="n">
-        <v>66666666</v>
+        <v>150000000</v>
       </c>
       <c r="S33" t="n">
-        <v>76666666</v>
+        <v>415000000</v>
       </c>
       <c r="AH33" t="n">
         <v>0.05</v>
@@ -1966,18 +1966,18 @@
         <v>1</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>GBP</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="Q34" t="n">
-        <v>66666666</v>
+        <v>150000000</v>
       </c>
       <c r="S34" t="n">
-        <v>143333333</v>
+        <v>415000000</v>
       </c>
       <c r="AH34" t="n">
         <v>0.05</v>
@@ -1991,18 +1991,18 @@
         <v>1</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>GBP</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="Q35" t="n">
-        <v>66666666</v>
+        <v>150000000</v>
       </c>
       <c r="S35" t="n">
-        <v>210000000</v>
+        <v>415000000</v>
       </c>
       <c r="AH35" t="n">
         <v>0.05</v>

</xml_diff>